<commit_message>
new sheet multiplying attack and defence rather than subtracting
</commit_message>
<xml_diff>
--- a/RelegatedTeams.xlsx
+++ b/RelegatedTeams.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackr\Documents\FPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{232DD4AE-2D67-4DC6-BAB2-AF85F7CC1EB2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B6FABD58-BB37-45EB-98C9-F9967EA9C6F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="0" windowWidth="18580" windowHeight="8540" xr2:uid="{21011593-3B87-4056-BC0C-D394C6C9EF32}"/>
+    <workbookView xWindow="1550" yWindow="0" windowWidth="18580" windowHeight="8540" activeTab="1" xr2:uid="{21011593-3B87-4056-BC0C-D394C6C9EF32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="diff goals" sheetId="3" r:id="rId1"/>
+    <sheet name="ratio goals" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="24">
   <si>
     <t>GF</t>
   </si>
@@ -329,12 +330,6 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -364,12 +359,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -386,6 +375,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,10 +700,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B83989-F5AF-43DC-BEC8-3CA22A3C0E94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6AE5A9-F7F5-4560-9D82-3547D6367CA8}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -715,625 +716,1284 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="23"/>
+      <c r="J1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="16" t="s">
+      <c r="L1" s="23"/>
+      <c r="M1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="17"/>
+      <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="15" t="s">
+      <c r="K2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>40</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>16</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>29</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>23</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="14">
         <v>-7.6315789473684295E-2</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="15">
         <v>-2.36842105263157E-2</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="14">
         <v>-0.81315789473684197</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="15">
         <v>0.186842105263157</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>40</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>17</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>39</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>29</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="14">
         <v>-0.49736842105263102</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="15">
         <v>-2.36842105263157E-2</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="14">
         <v>-0.70789473684210502</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="15">
         <v>0.39736842105263098</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>47</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>18</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>35</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>21</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>-0.28684210526315801</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="15">
         <v>2.89473684210526E-2</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>-0.44473684210526299</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="15">
         <v>0.23947368421052601</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>-0.44473684210526299</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="15">
         <v>-7.6315789473684295E-2</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>-0.76052631578947305</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="15">
         <v>0.34473684210526301</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>-0.28684210526315801</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="15">
         <v>0.23947368421052601</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="15">
         <v>0.66052631578947296</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="J8" s="13" t="s">
+      <c r="E8" s="23"/>
+      <c r="J8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="16">
         <v>-0.23421052631578901</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="17">
         <v>0.186842105263157</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="16">
         <v>-0.81315789473684197</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="17">
         <v>8.1578947368420904E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="22" t="s">
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="16">
         <f>AVERAGE(K3:K8)</f>
         <v>-0.30438596491228059</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="17">
         <f t="shared" ref="L9:N9" si="0">AVERAGE(L3:L8)</f>
         <v>5.5263157894736653E-2</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="16">
         <f t="shared" si="0"/>
         <v>-0.68157894736842095</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="17">
         <f t="shared" si="0"/>
         <v>0.31842105263157849</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <f>B3/23</f>
         <v>1.7391304347826086</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <f t="shared" ref="C10:E10" si="1">C3/23</f>
         <v>0.69565217391304346</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <f t="shared" si="1"/>
         <v>1.2608695652173914</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="14">
         <f t="shared" ref="B11:E12" si="2">B4/23</f>
         <v>1.7391304347826086</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="15">
         <f t="shared" si="2"/>
         <v>0.73913043478260865</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="14">
         <f t="shared" si="2"/>
         <v>1.6956521739130435</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="15">
         <f t="shared" si="2"/>
         <v>1.2608695652173914</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="16">
         <f t="shared" si="2"/>
         <v>2.0434782608695654</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <f t="shared" si="2"/>
         <v>0.78260869565217395</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="16">
         <f t="shared" si="2"/>
         <v>1.5217391304347827</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="17">
         <f t="shared" si="2"/>
         <v>0.91304347826086951</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="16" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="16" t="s">
+      <c r="L12" s="23"/>
+      <c r="M12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="17"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="15" t="s">
+      <c r="K13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="14">
         <f>(B24/2)+K$9</f>
         <v>-0.35511060259344013</v>
       </c>
-      <c r="L14" s="19">
-        <f t="shared" ref="L14:N14" si="3">(C24/2)+L$9</f>
+      <c r="L14" s="15">
+        <f t="shared" ref="L14:N16" si="3">(C24/2)+L$9</f>
         <v>3.3524027459954003E-2</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="14">
         <f t="shared" si="3"/>
         <v>-0.79752097635392805</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="15">
         <f t="shared" si="3"/>
         <v>0.28943554538520166</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="J15" s="12" t="s">
+      <c r="E15" s="23"/>
+      <c r="J15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="14">
         <f t="shared" ref="K15:K16" si="4">(B25/2)+K$9</f>
         <v>-0.35511060259344013</v>
       </c>
-      <c r="L15" s="19">
-        <f t="shared" ref="L15:L16" si="5">(C25/2)+L$9</f>
+      <c r="L15" s="15">
+        <f t="shared" si="3"/>
         <v>5.5263157894736653E-2</v>
       </c>
-      <c r="M15" s="18">
-        <f t="shared" ref="M15:M16" si="6">(D25/2)+M$9</f>
+      <c r="M15" s="14">
+        <f t="shared" si="3"/>
         <v>-0.58012967200610199</v>
       </c>
-      <c r="N15" s="19">
-        <f t="shared" ref="N15:N16" si="7">(E25/2)+N$9</f>
+      <c r="N15" s="15">
+        <f t="shared" si="3"/>
         <v>0.41987032799389734</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="B16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="16">
         <f t="shared" si="4"/>
         <v>-0.20293668954996175</v>
       </c>
-      <c r="L16" s="21">
-        <f t="shared" si="5"/>
+      <c r="L16" s="17">
+        <f t="shared" si="3"/>
         <v>7.7002288329519247E-2</v>
       </c>
-      <c r="M16" s="20">
-        <f t="shared" si="6"/>
+      <c r="M16" s="16">
+        <f t="shared" si="3"/>
         <v>-0.66708619374523237</v>
       </c>
-      <c r="N16" s="21">
-        <f t="shared" si="7"/>
+      <c r="N16" s="17">
+        <f t="shared" si="3"/>
         <v>0.24595728451563642</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="14">
         <f>B10-$K$22</f>
         <v>0.52807971014492749</v>
       </c>
-      <c r="C17" s="19">
-        <f t="shared" ref="C17:E17" si="8">C10-$K$22</f>
+      <c r="C17" s="15">
+        <f t="shared" ref="C17:E17" si="5">C10-$K$22</f>
         <v>-0.51539855072463769</v>
       </c>
-      <c r="D17" s="18">
-        <f t="shared" si="8"/>
+      <c r="D17" s="14">
+        <f t="shared" si="5"/>
         <v>4.98188405797102E-2</v>
       </c>
-      <c r="E17" s="19">
-        <f t="shared" si="8"/>
+      <c r="E17" s="15">
+        <f t="shared" si="5"/>
         <v>-0.21105072463768115</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="18">
-        <f t="shared" ref="B18:E18" si="9">B11-$K$22</f>
+      <c r="B18" s="14">
+        <f t="shared" ref="B18:E19" si="6">B11-$K$22</f>
         <v>0.52807971014492749</v>
       </c>
-      <c r="C18" s="19">
-        <f t="shared" si="9"/>
+      <c r="C18" s="15">
+        <f t="shared" si="6"/>
         <v>-0.47192028985507251</v>
       </c>
-      <c r="D18" s="18">
-        <f t="shared" si="9"/>
+      <c r="D18" s="14">
+        <f t="shared" si="6"/>
         <v>0.48460144927536231</v>
       </c>
-      <c r="E18" s="19">
-        <f t="shared" si="9"/>
+      <c r="E18" s="15">
+        <f t="shared" si="6"/>
         <v>4.98188405797102E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="20">
-        <f t="shared" ref="B19:E19" si="10">B12-$K$22</f>
+      <c r="B19" s="16">
+        <f t="shared" si="6"/>
         <v>0.83242753623188426</v>
       </c>
-      <c r="C19" s="21">
-        <f t="shared" si="10"/>
+      <c r="C19" s="17">
+        <f t="shared" si="6"/>
         <v>-0.42844202898550721</v>
       </c>
-      <c r="D19" s="20">
-        <f t="shared" si="10"/>
+      <c r="D19" s="16">
+        <f t="shared" si="6"/>
         <v>0.31068840579710155</v>
       </c>
-      <c r="E19" s="21">
-        <f t="shared" si="10"/>
+      <c r="E19" s="17">
+        <f t="shared" si="6"/>
         <v>-0.29800724637681164</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="1" t="s">
+      <c r="K20" s="21"/>
+      <c r="L20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="2"/>
+      <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="6">
         <v>1337</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21" s="6">
         <v>1018</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="23"/>
+      <c r="D22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="J22" s="9" t="s">
+      <c r="E22" s="23"/>
+      <c r="J22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="8">
         <f>K21/24/46</f>
         <v>1.2110507246376812</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="L22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="8">
         <f>M21/20/38</f>
         <v>1.3394736842105264</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15" t="s">
+      <c r="B23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="14">
         <f>B10-AVERAGE(B$10:B$12)</f>
         <v>-0.10144927536231907</v>
       </c>
-      <c r="C24" s="19">
-        <f t="shared" ref="C24:E24" si="11">C10-AVERAGE(C$10:C$12)</f>
+      <c r="C24" s="15">
+        <f t="shared" ref="C24:E24" si="7">C10-AVERAGE(C$10:C$12)</f>
         <v>-4.3478260869565299E-2</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="14">
+        <f t="shared" si="7"/>
+        <v>-0.23188405797101419</v>
+      </c>
+      <c r="E24" s="15">
+        <f t="shared" si="7"/>
+        <v>-5.7971014492753659E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="14">
+        <f t="shared" ref="B25:E26" si="8">B11-AVERAGE(B$10:B$12)</f>
+        <v>-0.10144927536231907</v>
+      </c>
+      <c r="C25" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="14">
+        <f t="shared" si="8"/>
+        <v>0.20289855072463792</v>
+      </c>
+      <c r="E25" s="15">
+        <f t="shared" si="8"/>
+        <v>0.20289855072463769</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="16">
+        <f t="shared" si="8"/>
+        <v>0.20289855072463769</v>
+      </c>
+      <c r="C26" s="17">
+        <f t="shared" si="8"/>
+        <v>4.3478260869565188E-2</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="8"/>
+        <v>2.8985507246377162E-2</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="8"/>
+        <v>-0.14492753623188415</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B83989-F5AF-43DC-BEC8-3CA22A3C0E94}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="J1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="23"/>
+      <c r="M1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2">
+        <v>23</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="14">
+        <v>0.94</v>
+      </c>
+      <c r="L3" s="15">
+        <v>0.98</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0.39</v>
+      </c>
+      <c r="N3" s="15">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2">
+        <v>29</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0.63</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0.98</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0.47</v>
+      </c>
+      <c r="N4" s="15">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4">
+        <v>21</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.79</v>
+      </c>
+      <c r="L5" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="N5" s="15">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0.79</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1.18</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.59</v>
+      </c>
+      <c r="N6" s="15">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0.94</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0.43</v>
+      </c>
+      <c r="N7" s="15">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="J8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.83</v>
+      </c>
+      <c r="L8" s="17">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.39</v>
+      </c>
+      <c r="N8" s="17">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="16">
+        <f>AVERAGE(K3:K8)</f>
+        <v>0.77499999999999991</v>
+      </c>
+      <c r="L9" s="17">
+        <f t="shared" ref="L9:N9" si="0">AVERAGE(L3:L8)</f>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="M9" s="16">
+        <f t="shared" si="0"/>
+        <v>0.49000000000000005</v>
+      </c>
+      <c r="N9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2383333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="14">
+        <f>B3/23</f>
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="C10" s="15">
+        <f t="shared" ref="C10:E10" si="1">C3/23</f>
+        <v>0.69565217391304346</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2608695652173914</v>
+      </c>
+      <c r="E10" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14">
+        <f t="shared" ref="B11:E12" si="2">B4/23</f>
+        <v>1.7391304347826086</v>
+      </c>
+      <c r="C11" s="15">
+        <f t="shared" si="2"/>
+        <v>0.73913043478260865</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="2"/>
+        <v>1.6956521739130435</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2608695652173914</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" si="2"/>
+        <v>2.0434782608695654</v>
+      </c>
+      <c r="C12" s="17">
+        <f t="shared" si="2"/>
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="D12" s="16">
+        <f t="shared" si="2"/>
+        <v>1.5217391304347827</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="2"/>
+        <v>0.91304347826086951</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="14">
+        <f>B24*K$9</f>
+        <v>0.73228346456692894</v>
+      </c>
+      <c r="L14" s="15">
+        <f t="shared" ref="L14:N14" si="3">C24*L$9</f>
+        <v>0.97882352941176443</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="3"/>
+        <v>0.41388349514563122</v>
+      </c>
+      <c r="N14" s="15">
+        <f t="shared" si="3"/>
+        <v>1.1704794520547945</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="J15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="14">
+        <f t="shared" ref="K15:K16" si="4">B25*K$9</f>
+        <v>0.73228346456692894</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" ref="L15:L16" si="5">C25*L$9</f>
+        <v>1.0399999999999996</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" ref="M15:M16" si="6">D25*M$9</f>
+        <v>0.55660194174757294</v>
+      </c>
+      <c r="N15" s="15">
+        <f t="shared" ref="N15:N16" si="7">E25*N$9</f>
+        <v>1.4758219178082193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="16">
+        <f t="shared" si="4"/>
+        <v>0.86043307086614162</v>
+      </c>
+      <c r="L16" s="17">
+        <f t="shared" si="5"/>
+        <v>1.1011764705882352</v>
+      </c>
+      <c r="M16" s="16">
+        <f t="shared" si="6"/>
+        <v>0.49951456310679626</v>
+      </c>
+      <c r="N16" s="17">
+        <f t="shared" si="7"/>
+        <v>1.0686986301369861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="14">
+        <f>B10/$K$22</f>
+        <v>1.4360508601346298</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" ref="C17:E17" si="8">C10/$K$22</f>
+        <v>0.57442034405385189</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="8"/>
+        <v>1.0411368735976065</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="8"/>
+        <v>0.82572924457741215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="14">
+        <f t="shared" ref="B18:E18" si="9">B11/$K$22</f>
+        <v>1.4360508601346298</v>
+      </c>
+      <c r="C18" s="15">
+        <f t="shared" si="9"/>
+        <v>0.61032161555721764</v>
+      </c>
+      <c r="D18" s="14">
+        <f t="shared" si="9"/>
+        <v>1.400149588631264</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="9"/>
+        <v>1.0411368735976065</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="16">
+        <f t="shared" ref="B19:E19" si="10">B12/$K$22</f>
+        <v>1.68735976065819</v>
+      </c>
+      <c r="C19" s="17">
+        <f t="shared" si="10"/>
+        <v>0.6462228870605834</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="10"/>
+        <v>1.256544502617801</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" si="10"/>
+        <v>0.75392670157068054</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J20" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="21"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1337</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="J22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="8">
+        <f>K21/24/46</f>
+        <v>1.2110507246376812</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="8">
+        <f>M21/20/38</f>
+        <v>1.3394736842105264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="14">
+        <f>B10/AVERAGE(B$10:B$12)</f>
+        <v>0.9448818897637794</v>
+      </c>
+      <c r="C24" s="15">
+        <f t="shared" ref="C24:E24" si="11">C10/AVERAGE(C$10:C$12)</f>
+        <v>0.94117647058823517</v>
+      </c>
+      <c r="D24" s="14">
         <f t="shared" si="11"/>
-        <v>-0.23188405797101419</v>
-      </c>
-      <c r="E24" s="19">
+        <v>0.84466019417475746</v>
+      </c>
+      <c r="E24" s="15">
         <f t="shared" si="11"/>
-        <v>-5.7971014492753659E-2</v>
+        <v>0.9452054794520548</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="18">
-        <f t="shared" ref="B25:E26" si="12">B11-AVERAGE(B$10:B$12)</f>
-        <v>-0.10144927536231907</v>
-      </c>
-      <c r="C25" s="19">
+      <c r="B25" s="14">
+        <f t="shared" ref="B25:E25" si="12">B11/AVERAGE(B$10:B$12)</f>
+        <v>0.9448818897637794</v>
+      </c>
+      <c r="C25" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="18">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D25" s="14">
         <f t="shared" si="12"/>
-        <v>0.20289855072463792</v>
-      </c>
-      <c r="E25" s="19">
+        <v>1.1359223300970875</v>
+      </c>
+      <c r="E25" s="15">
         <f t="shared" si="12"/>
-        <v>0.20289855072463769</v>
+        <v>1.1917808219178083</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="20">
-        <f t="shared" si="12"/>
-        <v>0.20289855072463769</v>
-      </c>
-      <c r="C26" s="21">
-        <f t="shared" si="12"/>
-        <v>4.3478260869565188E-2</v>
-      </c>
-      <c r="D26" s="20">
-        <f t="shared" si="12"/>
-        <v>2.8985507246377162E-2</v>
-      </c>
-      <c r="E26" s="21">
-        <f t="shared" si="12"/>
-        <v>-0.14492753623188415</v>
+      <c r="B26" s="16">
+        <f t="shared" ref="B26:E26" si="13">B12/AVERAGE(B$10:B$12)</f>
+        <v>1.110236220472441</v>
+      </c>
+      <c r="C26" s="17">
+        <f t="shared" si="13"/>
+        <v>1.0588235294117647</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="13"/>
+        <v>1.0194174757281556</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="13"/>
+        <v>0.86301369863013688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>